<commit_message>
Integrated generation and done some UI/UX tweaks
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,6 +579,72 @@
       </c>
       <c r="I4" t="inlineStr"/>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Allam</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>allam@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>pbkdf2:sha256:260000$jhqElP07ppJlhh3v$8e6af83a284632ae86d6b2c5f430b6b0efd7e235db92dbca4e9b7793331b61c8</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-06-26T21:36:13.811742</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Allam1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>allam100@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Allam123@</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-06-27T02:08:49.212447</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>